<commit_message>
fixed the inverted trend and cluster logic
</commit_message>
<xml_diff>
--- a/RELIANCE.NS_adaptive_supertrend.xlsx
+++ b/RELIANCE.NS_adaptive_supertrend.xlsx
@@ -29718,10 +29718,10 @@
         <v>45756</v>
       </c>
       <c r="B476" t="n">
-        <v>1185.949951171875</v>
+        <v>1185.099975585938</v>
       </c>
       <c r="C476" t="n">
-        <v>1185.949951171875</v>
+        <v>1185.099975585938</v>
       </c>
       <c r="D476" t="n">
         <v>1189.800048828125</v>
@@ -29733,7 +29733,7 @@
         <v>1169.5</v>
       </c>
       <c r="G476" t="n">
-        <v>4565534</v>
+        <v>4580862</v>
       </c>
       <c r="H476" t="n">
         <v>32.49998779296875</v>

</xml_diff>